<commit_message>
Encoders implemented on Arduino, ticks implemented on beagle. Removed legacy communication code from Arduino library. Updated Arduino library to v1.0. Misc. bug fixes
</commit_message>
<xml_diff>
--- a/doc/SerialDataFormat.xlsx
+++ b/doc/SerialDataFormat.xlsx
@@ -12,16 +12,16 @@
     <sheet name="RSL(0)" sheetId="7" r:id="rId3"/>
     <sheet name="PWM(1)" sheetId="3" r:id="rId4"/>
     <sheet name="DigitalIO(2)" sheetId="4" r:id="rId5"/>
-    <sheet name="Encoder(4)" sheetId="5" r:id="rId6"/>
-    <sheet name="AnalogIO(3)" sheetId="6" r:id="rId7"/>
-    <sheet name="DutyCycle(4)" sheetId="8" r:id="rId8"/>
+    <sheet name="AnalogIO(3)" sheetId="6" r:id="rId6"/>
+    <sheet name="DutyCycle(4)" sheetId="8" r:id="rId7"/>
+    <sheet name="Encoder(5)" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
   <si>
     <t>Header</t>
   </si>
@@ -149,15 +149,6 @@
     <t>Ticks</t>
   </si>
   <si>
-    <t>flags</t>
-  </si>
-  <si>
-    <t>ResetTickCount/Invert/possibly other flags</t>
-  </si>
-  <si>
-    <t>echoed from command</t>
-  </si>
-  <si>
     <t>int64</t>
   </si>
   <si>
@@ -183,6 +174,12 @@
   </si>
   <si>
     <t>Staet</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>0 - ok, 1 - fail</t>
   </si>
 </sst>
 </file>
@@ -244,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -271,6 +268,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,7 +926,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1156,7 +1159,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1221,7 +1224,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1233,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,228 +1351,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f>E3+D3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <f>E5+D5</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E8" si="0">E6+D6</f>
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <f>E11+D11</f>
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <f>E13+D13</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <f t="shared" ref="E15" si="1">E14+D14</f>
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="B12:F12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1612,7 +1393,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1626,7 +1407,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1650,7 +1431,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -1663,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,7 +1485,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
@@ -1718,7 +1499,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1775,12 +1556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1691,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1921,4 +1702,215 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>E3+D3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>E5+D5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" ref="E7:E8" si="0">E6+D6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f>E11+D13</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <f>E13+D14</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f>E14+D15</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="B12:F12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on UdpProxy. Kiwi demo almost drivable. Implementing velocity PID.
</commit_message>
<xml_diff>
--- a/doc/SerialDataFormat.xlsx
+++ b/doc/SerialDataFormat.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SerialPacketing" sheetId="1" r:id="rId1"/>
     <sheet name="IOCommandData" sheetId="2" r:id="rId2"/>
     <sheet name="RSL(0)" sheetId="7" r:id="rId3"/>
-    <sheet name="PWM(1)" sheetId="3" r:id="rId4"/>
-    <sheet name="DigitalIO(2)" sheetId="4" r:id="rId5"/>
-    <sheet name="AnalogIO(3)" sheetId="6" r:id="rId6"/>
-    <sheet name="DutyCycle(4)" sheetId="8" r:id="rId7"/>
-    <sheet name="Encoder(5)" sheetId="5" r:id="rId8"/>
+    <sheet name="Sections" sheetId="9" r:id="rId4"/>
+    <sheet name="PWM(1)" sheetId="3" r:id="rId5"/>
+    <sheet name="DigitalIO(2)" sheetId="4" r:id="rId6"/>
+    <sheet name="AnalogIO(3)" sheetId="6" r:id="rId7"/>
+    <sheet name="DutyCycle(4)" sheetId="8" r:id="rId8"/>
+    <sheet name="Encoder(5)" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="70">
   <si>
     <t>Header</t>
   </si>
@@ -180,6 +181,57 @@
   </si>
   <si>
     <t>0 - ok, 1 - fail</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Udp</t>
+  </si>
+  <si>
+    <t>Universal</t>
+  </si>
+  <si>
+    <t>RslSection</t>
+  </si>
+  <si>
+    <t>StateSection</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t>AIO</t>
+  </si>
+  <si>
+    <t>AnalogIOSection</t>
+  </si>
+  <si>
+    <t>DigitalIOSection</t>
+  </si>
+  <si>
+    <t>DutyCycle</t>
+  </si>
+  <si>
+    <t>DutyCycleSection</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>EncoderSection</t>
+  </si>
+  <si>
+    <t>PWM/Motor</t>
+  </si>
+  <si>
+    <t>PwmSection</t>
+  </si>
+  <si>
+    <t>MotorSection</t>
   </si>
 </sst>
 </file>
@@ -257,6 +309,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -268,12 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,13 +660,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -667,13 +719,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -689,7 +741,7 @@
         <f>D5+C5</f>
         <v>8</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -707,7 +759,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -723,7 +775,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -739,7 +791,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -755,7 +807,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -800,13 +852,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -823,13 +875,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -898,14 +950,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1019,6 +1071,215 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1035,14 +1296,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1076,13 +1337,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1127,14 +1388,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1180,7 +1441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -1196,14 +1457,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1350,7 +1611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1365,14 +1626,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1406,13 +1667,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1457,14 +1718,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1498,13 +1759,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1556,7 +1817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1567,14 +1828,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1608,13 +1869,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1659,14 +1920,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1704,11 +1965,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1720,14 +1981,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1761,13 +2022,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1812,14 +2073,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1853,29 +2114,29 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="10">
         <v>1</v>
       </c>
       <c r="E13">
         <f>E11+D13</f>
         <v>1</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="9" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementing multi-sample analog IO. -Needed to reduce Gyro drift.
Noticed RAM usage issues on Arduino.
-Need to do reduce RAM load, and identify the source(s) of it's usage.
</commit_message>
<xml_diff>
--- a/doc/SerialDataFormat.xlsx
+++ b/doc/SerialDataFormat.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SerialPacketing" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="75">
   <si>
     <t>Header</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Samples</t>
   </si>
   <si>
-    <t>Number of sample to average, may not get implemented</t>
-  </si>
-  <si>
     <t>Each bit sit high if the respectiev pin state should be set or retreived</t>
   </si>
   <si>
@@ -232,13 +229,54 @@
   </si>
   <si>
     <t>MotorSection</t>
+  </si>
+  <si>
+    <t>Minimum delay between samples, may not be slower than communication reate</t>
+  </si>
+  <si>
+    <t>AIOSample</t>
+  </si>
+  <si>
+    <r>
+      <t>Samples[</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Samples</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Delay since previous sample</t>
+  </si>
+  <si>
+    <t>MinSampleInterval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +286,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -978,7 +1024,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1074,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,19 +1133,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,13 +1153,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,13 +1167,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1135,10 +1181,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,10 +1192,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
         <v>60</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,10 +1203,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
         <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,10 +1214,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
         <v>65</v>
-      </c>
-      <c r="E7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,7 +1531,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1497,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1613,16 +1659,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,10 +1739,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1705,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1784,13 +1831,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f>E13+D13</f>
@@ -1798,22 +1845,58 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <f t="shared" ref="E15" si="1">E14+D14</f>
-        <v>4</v>
+      <c r="B15" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f>E16+D16</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2124,7 +2207,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>26</v>
@@ -2137,7 +2220,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>